<commit_message>
Bugfixes for the callerscripts
continued visualization
</commit_message>
<xml_diff>
--- a/techniques_greenred.xlsx
+++ b/techniques_greenred.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Internship\gitrepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D78CCAE-E908-4290-B513-E65BB91C6C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B1FE3A-D880-4D2C-8B43-EBDC6EA94863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4665" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38175" yWindow="7395" windowWidth="16575" windowHeight="8670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>split /classification</t>
   </si>
@@ -55,6 +55,45 @@
   </si>
   <si>
     <t>SCA</t>
+  </si>
+  <si>
+    <t>Original Data</t>
+  </si>
+  <si>
+    <t>kmcluster</t>
+  </si>
+  <si>
+    <t>dbscan</t>
+  </si>
+  <si>
+    <t>forest</t>
+  </si>
+  <si>
+    <t>Preprocessing</t>
+  </si>
+  <si>
+    <t>Datamerging</t>
+  </si>
+  <si>
+    <t>Preprocessing AE</t>
+  </si>
+  <si>
+    <t>Baselines</t>
+  </si>
+  <si>
+    <t>START: 04 49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">END 05 05 </t>
+  </si>
+  <si>
+    <t>Autoencoders</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -70,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,8 +134,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -141,6 +186,32 @@
       <right style="thick">
         <color auto="1"/>
       </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -148,10 +219,36 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thick">
@@ -163,21 +260,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top/>
@@ -187,8 +273,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thin">
@@ -200,8 +288,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thin">
@@ -213,27 +303,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -241,54 +344,263 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thick">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,86 +881,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D13"/>
+  <dimension ref="B5:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="6"/>
-      <c r="C4" s="1" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="33">
+        <v>10</v>
+      </c>
+      <c r="E5" s="32">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="32"/>
+      <c r="C6" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="33">
+        <v>26</v>
+      </c>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="32"/>
+      <c r="C7" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="33">
+        <v>30</v>
+      </c>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="33">
+        <v>16</v>
+      </c>
+      <c r="E8" s="32">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
+      <c r="C9" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="33">
+        <v>16</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="32"/>
+      <c r="C10" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="33">
+        <v>3</v>
+      </c>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="32"/>
+      <c r="C11" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="33">
+        <v>32</v>
+      </c>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="32"/>
+      <c r="C12" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="33">
+        <v>8</v>
+      </c>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="32"/>
+      <c r="C14" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="33"/>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="32"/>
+      <c r="C15" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="33"/>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="6"/>
+      <c r="C19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="E19" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="C20" s="7"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="18">
+        <v>1</v>
+      </c>
+      <c r="F20" s="19">
+        <v>72</v>
+      </c>
+      <c r="G20" s="20">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="C21" s="8"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11">
+        <v>81</v>
+      </c>
+      <c r="G21" s="12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="C22" s="8"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="21">
+        <v>1</v>
+      </c>
+      <c r="F22" s="11">
+        <v>6</v>
+      </c>
+      <c r="G22" s="12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="C23" s="8"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="21">
+        <v>1</v>
+      </c>
+      <c r="F23" s="11">
+        <v>3</v>
+      </c>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="C24" s="8"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="21">
+        <v>0</v>
+      </c>
+      <c r="F24" s="11">
+        <v>5</v>
+      </c>
+      <c r="G24" s="12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
+      <c r="C26" s="8"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="21">
+        <v>1</v>
+      </c>
+      <c r="F26" s="11">
+        <v>30</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26">
+        <v>1</v>
+      </c>
+      <c r="F27" s="27">
+        <v>6</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="22">
+        <v>5</v>
+      </c>
+      <c r="F28" s="34">
+        <v>631</v>
+      </c>
+      <c r="G28" s="13">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="B13:B15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
finished up the pipeline: now it's on to evaluate them:
</commit_message>
<xml_diff>
--- a/techniques_greenred.xlsx
+++ b/techniques_greenred.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Internship\gitrepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13979214-07C1-4CB9-B660-2D4FB6EB3BC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6E2EB6-BA59-41A2-9758-01163CBDCB27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38175" yWindow="7395" windowWidth="16575" windowHeight="8670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -878,7 +878,7 @@
   <dimension ref="B5:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="B5:E15"/>
+      <selection activeCell="E13" sqref="E13:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,7 +983,9 @@
       <c r="C13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="32"/>
+      <c r="D13" s="32">
+        <v>117</v>
+      </c>
       <c r="E13" s="34"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -991,7 +993,9 @@
       <c r="C14" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="32"/>
+      <c r="D14" s="32">
+        <v>143</v>
+      </c>
       <c r="E14" s="34"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -999,7 +1003,9 @@
       <c r="C15" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" s="32">
+        <v>43</v>
+      </c>
       <c r="E15" s="34"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>